<commit_message>
update the software context and API's as covered and every API took specific id
Signed-off-by: bassem ezzat <bassem.ezzat1993@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
+++ b/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0693AEDF-2B98-40F6-8B86-B4742A58272B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2412" yWindow="3168" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="3165" windowWidth="17280" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -161,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -532,12 +531,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -549,46 +581,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -707,7 +706,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -742,7 +741,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -919,210 +918,227 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="32">
+      <c r="C9" s="33"/>
+      <c r="D9" s="31">
         <v>43864</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="32">
+      <c r="D13" s="24"/>
+      <c r="E13" s="31">
         <v>43864</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1139,23 +1155,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1163,27 +1162,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
@@ -1231,11 +1230,13 @@
       <c r="F2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
@@ -1248,11 +1249,13 @@
       <c r="F3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>44076</v>
       </c>
@@ -1383,7 +1386,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -1446,7 +1449,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -1463,7 +1466,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
@@ -1480,7 +1483,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -1497,7 +1500,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
@@ -1514,7 +1517,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
@@ -1531,7 +1534,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
@@ -1565,7 +1568,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1576,7 +1579,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1587,7 +1590,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1598,7 +1601,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1609,7 +1612,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1620,7 +1623,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1631,7 +1634,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
@@ -1642,7 +1645,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1653,7 +1656,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1664,7 +1667,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1675,7 +1678,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1686,7 +1689,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1697,7 +1700,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1708,7 +1711,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1719,7 +1722,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1730,7 +1733,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1741,7 +1744,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1752,7 +1755,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1763,7 +1766,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1774,7 +1777,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1785,7 +1788,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1796,7 +1799,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1807,7 +1810,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1818,7 +1821,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1829,7 +1832,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1840,7 +1843,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1851,7 +1854,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -1884,10 +1887,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated the review sheet of GDD Signed-off-by: ghada <C:Usersghadasw_software_engineer>
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
+++ b/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2F7472-A099-494E-9E18-3049C90F0C57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="3165" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -103,24 +104,12 @@
     <t xml:space="preserve">Is for the reviewer he check the fix of the open point and check if the fix is ok or still open </t>
   </si>
   <si>
-    <t>T.Sharaby</t>
-  </si>
-  <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t>30/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V0.1 </t>
-  </si>
-  <si>
     <t>PO3_DGW</t>
   </si>
   <si>
-    <t>V0.4</t>
-  </si>
-  <si>
     <t>Mariam</t>
   </si>
   <si>
@@ -142,9 +131,6 @@
     <t>GDD</t>
   </si>
   <si>
-    <t>SRS</t>
-  </si>
-  <si>
     <t>V0.1</t>
   </si>
   <si>
@@ -155,12 +141,39 @@
   </si>
   <si>
     <t>All documents named "PO3_DGW_GDD", but the name of this document name "DGW_PO3_GDD"</t>
+  </si>
+  <si>
+    <t>V0.0</t>
+  </si>
+  <si>
+    <t>page7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moahmed </t>
+  </si>
+  <si>
+    <t>adding software feature</t>
+  </si>
+  <si>
+    <t>adding the signals in the contex digram</t>
+  </si>
+  <si>
+    <t>Ghada</t>
+  </si>
+  <si>
+    <t>in descrirtion of API breif description</t>
+  </si>
+  <si>
+    <t>return value of the error must be clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">section for the API for each commponent </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -531,12 +544,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,43 +594,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -918,227 +931,210 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D7" sqref="D7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="32" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="31">
+      <c r="C9" s="25"/>
+      <c r="D9" s="32">
         <v>43864</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
-    </row>
-    <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35" t="s">
+      <c r="C12" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="36"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="31">
+      <c r="C13" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="32">
         <v>43864</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1155,6 +1151,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1162,27 +1175,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
-    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" customWidth="1"/>
+    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1211,24 +1224,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>28</v>
-      </c>
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>29</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C2" s="13"/>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>19</v>
@@ -1236,18 +1245,18 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
       <c r="D3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>19</v>
@@ -1255,16 +1264,10 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
@@ -1275,16 +1278,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
       <c r="F5" s="23"/>
@@ -1295,16 +1292,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
       <c r="F6" s="11"/>
@@ -1312,16 +1303,10 @@
       <c r="H6" s="10"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
@@ -1332,16 +1317,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
@@ -1352,16 +1331,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>29</v>
-      </c>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
@@ -1369,16 +1342,10 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>44076</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
@@ -1386,15 +1353,15 @@
       <c r="H10" s="10"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -1409,15 +1376,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -1432,15 +1399,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -1449,15 +1416,15 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -1466,15 +1433,15 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -1483,15 +1450,15 @@
       <c r="H15" s="10"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="17"/>
@@ -1500,15 +1467,15 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="17"/>
@@ -1517,15 +1484,15 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="20"/>
@@ -1534,15 +1501,15 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="20"/>
@@ -1551,15 +1518,15 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="20"/>
@@ -1568,62 +1535,116 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>43985</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>43985</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="7"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>43985</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>43985</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="7"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>43985</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1634,7 +1655,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
@@ -1645,7 +1666,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1656,7 +1677,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1667,7 +1688,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1678,7 +1699,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1689,7 +1710,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1700,7 +1721,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1711,7 +1732,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1722,7 +1743,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1733,7 +1754,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1744,7 +1765,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1755,7 +1776,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1766,7 +1787,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1777,7 +1798,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1788,7 +1809,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1799,7 +1820,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1810,7 +1831,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1821,7 +1842,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1832,7 +1853,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1843,7 +1864,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1854,7 +1875,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -1887,10 +1908,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Signed-off-by: bassem ezzat <bassem.ezzat1993@gmail.com> review after adding software features
Signed-off-by: bassem ezzat <bassem.ezzat1993@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
+++ b/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2F7472-A099-494E-9E18-3049C90F0C57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3090" windowWidth="17280" windowHeight="8910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
     <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc30697436" localSheetId="1">'Cross review points '!$F$7</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">'Cross review points '!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -80,24 +79,9 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Accepted</t>
   </si>
   <si>
-    <t>Refused</t>
-  </si>
-  <si>
-    <t>Resolved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision </t>
-  </si>
-  <si>
-    <t xml:space="preserve">whether to accept the open point if you see applicable and valid or to refuse it and give a justification in the comment field whether you accept , then update with the action you did , or refuse with justification </t>
-  </si>
-  <si>
     <t xml:space="preserve">Status </t>
   </si>
   <si>
@@ -110,70 +94,55 @@
     <t>PO3_DGW</t>
   </si>
   <si>
-    <t>Mariam</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>28/2/2020</t>
-  </si>
-  <si>
-    <t>V0.5</t>
-  </si>
-  <si>
-    <t>Page 6</t>
-  </si>
-  <si>
-    <t>software context should be as blocks (input and output)</t>
-  </si>
-  <si>
     <t>GDD</t>
   </si>
   <si>
-    <t>V0.1</t>
-  </si>
-  <si>
     <t>Mohammed Elsayed</t>
   </si>
   <si>
     <t>page 1</t>
   </si>
   <si>
-    <t>All documents named "PO3_DGW_GDD", but the name of this document name "DGW_PO3_GDD"</t>
-  </si>
-  <si>
     <t>V0.0</t>
   </si>
   <si>
-    <t>page7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moahmed </t>
-  </si>
-  <si>
-    <t>adding software feature</t>
-  </si>
-  <si>
-    <t>adding the signals in the contex digram</t>
-  </si>
-  <si>
-    <t>Ghada</t>
-  </si>
-  <si>
-    <t>in descrirtion of API breif description</t>
-  </si>
-  <si>
-    <t>return value of the error must be clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section for the API for each commponent </t>
+    <t>Bassem Ezzat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">review to GDD after adding software features </t>
+  </si>
+  <si>
+    <t>Bassem</t>
+  </si>
+  <si>
+    <t>Page 8</t>
+  </si>
+  <si>
+    <t>API's tables should be classified into separate component sectors.</t>
+  </si>
+  <si>
+    <t>Api's error_t should be clear.</t>
+  </si>
+  <si>
+    <t>page 7</t>
+  </si>
+  <si>
+    <t>physical range coulom in input/output table is out of GDD scope</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>software feature should be more detailed and use the signal from input/output table.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -479,7 +448,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -541,9 +510,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,8 +565,8 @@
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -931,207 +897,215 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:H7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="28"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+    </row>
+    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="32">
-        <v>43864</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="31">
+        <v>44015</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="C12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="32">
+      <c r="C13" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="31">
         <v>43864</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="31">
+        <v>44046</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -1175,27 +1149,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1224,86 +1198,111 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>44046</v>
+      </c>
       <c r="B2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="13"/>
+        <v>30</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D2" s="7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>19</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>44046</v>
+      </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D3" s="7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>19</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>44046</v>
+      </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="K4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>44046</v>
+      </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="23"/>
+      <c r="C5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -1313,11 +1312,8 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="12"/>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
@@ -1327,11 +1323,8 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="12"/>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1342,175 +1335,109 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="12"/>
-      <c r="K11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="12"/>
-      <c r="K12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="7"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="18"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="7"/>
       <c r="E19" s="20"/>
       <c r="F19" s="21"/>
@@ -1518,16 +1445,10 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7"/>
       <c r="E20" s="20"/>
       <c r="F20" s="21"/>
@@ -1535,152 +1456,98 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>43985</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>42</v>
-      </c>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>43985</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>43</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>43985</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21" t="s">
-        <v>45</v>
-      </c>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>43985</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>34</v>
-      </c>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="F24" s="21"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>43985</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>34</v>
-      </c>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="F25" s="22"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="17"/>
       <c r="F29" s="21"/>
@@ -1688,29 +1555,29 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="16"/>
-      <c r="E30" s="20"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="22"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1721,7 +1588,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1732,18 +1599,18 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="20"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1754,7 +1621,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1765,7 +1632,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1776,7 +1643,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1787,7 +1654,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1798,7 +1665,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1809,7 +1676,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1819,72 +1686,6 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="19"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="19"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="19"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -1908,11 +1709,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>$K$4:$K$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>$K$4:$K$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>$K$7:$K$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename GDD document cover review point. modified review document format.
</commit_message>
<xml_diff>
--- a/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
+++ b/Software Specification/Architecture/GDD/PO3_DGW_GDD_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B864451D-8737-49D9-8417-3095297F0829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3090" windowWidth="17280" windowHeight="8910" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -137,12 +138,21 @@
   </si>
   <si>
     <t>software feature should be more detailed and use the signal from input/output table.</t>
+  </si>
+  <si>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -510,12 +520,45 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,46 +570,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -897,218 +907,235 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="28"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="28"/>
-    </row>
-    <row r="6" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="23" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="23" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="31">
+      <c r="C9" s="32"/>
+      <c r="D9" s="30">
         <v>44015</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="31">
+      <c r="D13" s="23"/>
+      <c r="E13" s="30">
         <v>43864</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="31">
+      <c r="D14" s="23"/>
+      <c r="E14" s="30">
         <v>44046</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29" t="s">
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1125,23 +1152,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1149,27 +1159,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
-    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" customWidth="1"/>
+    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>44046</v>
       </c>
@@ -1217,15 +1227,19 @@
       <c r="F2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>44046</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="13" t="s">
         <v>36</v>
       </c>
@@ -1238,15 +1252,21 @@
       <c r="F3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>44046</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" s="13" t="s">
         <v>36</v>
       </c>
@@ -1257,18 +1277,24 @@
       <c r="F4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="I4" s="10"/>
       <c r="K4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>44046</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="13" t="s">
         <v>36</v>
       </c>
@@ -1281,11 +1307,18 @@
       <c r="F5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -1302,7 +1335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13"/>
@@ -1312,8 +1345,11 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="13"/>
@@ -1323,8 +1359,11 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1335,7 +1374,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1346,7 +1385,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1357,7 +1396,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1368,7 +1407,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1379,7 +1418,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1390,7 +1429,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
@@ -1401,7 +1440,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
@@ -1412,7 +1451,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1423,7 +1462,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1434,7 +1473,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1445,7 +1484,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1456,7 +1495,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1467,7 +1506,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1478,7 +1517,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1489,7 +1528,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1500,7 +1539,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1511,7 +1550,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1522,7 +1561,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1533,7 +1572,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1544,7 +1583,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1555,7 +1594,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1566,7 +1605,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1577,7 +1616,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1588,7 +1627,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1599,7 +1638,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1610,7 +1649,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1621,7 +1660,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1632,7 +1671,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1643,7 +1682,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1654,7 +1693,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1665,7 +1704,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1676,7 +1715,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1709,11 +1748,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
-      <formula1>$K$4:$K$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
-      <formula1>#REF!</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>